<commit_message>
Updates to profile pages, publication pages
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Erika_Freeman/Author_form.xlsx
+++ b/website_content_creation/authors/Erika_Freeman/Author_form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\Documents\WET lab\WETlab_website\website_content_creation\Erika_Freeman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\Documents\WET lab\WETlab_website\website_content_creation\authors\Erika_Freeman\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -41,9 +41,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>PhD Student</t>
-  </si>
-  <si>
     <t>Twitter</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>BSc Environmental Science, Geographic Information Science (coop)</t>
   </si>
   <si>
-    <t>Organizations</t>
-  </si>
-  <si>
     <t>Organization_name</t>
   </si>
   <si>
@@ -150,6 +144,18 @@
   </si>
   <si>
     <t>Visiting and Co-supervised Students</t>
+  </si>
+  <si>
+    <t>PhD Student, Cambridge University</t>
+  </si>
+  <si>
+    <t>Academic Supervisor (for students)</t>
+  </si>
+  <si>
+    <t>Andrew Tanentzap</t>
+  </si>
+  <si>
+    <t>Organizations (include academic institution or lab if you are a student)</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -406,11 +412,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -446,12 +465,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:C1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -703,170 +728,174 @@
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
+      <c r="B4" s="29" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-    </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C17" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="16">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="16">
+      <c r="B18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="16">
         <v>2016</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="28"/>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="27"/>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B24" s="20" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
@@ -880,34 +909,37 @@
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
     </row>
     <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
     </row>
-    <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18"/>
+    </row>
     <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1871,18 +1903,19 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B23" r:id="rId4"/>
-    <hyperlink ref="B24" r:id="rId5"/>
-    <hyperlink ref="B25" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="B24" r:id="rId4"/>
+    <hyperlink ref="B25" r:id="rId5"/>
+    <hyperlink ref="B26" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>